<commit_message>
Data for Exercise 6.13.
</commit_message>
<xml_diff>
--- a/data/Exercise6.13.xlsx
+++ b/data/Exercise6.13.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Applied-Multivariate-Statistical-Analysis-Solutions\Applied-Multivariate-Statistical-Analysis-Solutions\Applied-Multivariate-Statistical-Analysis-Solutions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DF8080-D2CA-4420-AD0D-8B7446EDBB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE941B6-4244-46AB-AA8E-CA5B5D6EBB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0C7D62E-A11B-4AD5-B25C-4573E1B7FC7C}"/>
+    <workbookView xWindow="6030" yWindow="2310" windowWidth="21600" windowHeight="11385" xr2:uid="{B0C7D62E-A11B-4AD5-B25C-4573E1B7FC7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>